<commit_message>
Dados de segurança analisados
</commit_message>
<xml_diff>
--- a/br_inep_ideb.xlsx
+++ b/br_inep_ideb.xlsx
@@ -203,8 +203,8 @@
   </sheetPr>
   <dimension ref="A1:K127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A93" activeCellId="0" sqref="93:93"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="9:9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -213,6 +213,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="32.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>